<commit_message>
seems to work, going to try in scenarios
</commit_message>
<xml_diff>
--- a/tests/testpwid.xlsx
+++ b/tests/testpwid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1094,17 +1094,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="67" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="250">
@@ -1668,15 +1668,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="61"/>
+      <c r="A2" s="63"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="61"/>
+      <c r="A3" s="63"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="28"/>
@@ -1712,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2495,9 +2495,7 @@
       <c r="X29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y29" s="4">
-        <v>0</v>
-      </c>
+      <c r="Y29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2514,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2583,7 +2581,9 @@
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -2591,7 +2591,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2622,7 +2622,9 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="3" t="str">
@@ -2783,7 +2785,9 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="3" t="str">
@@ -3087,7 +3091,9 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
@@ -3321,7 +3327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
@@ -13773,7 +13779,7 @@
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
-      <c r="P45" s="62">
+      <c r="P45" s="60">
         <v>1E-3</v>
       </c>
       <c r="Q45" s="9"/>
@@ -14109,8 +14115,8 @@
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
-      <c r="L58" s="63"/>
-      <c r="M58" s="63"/>
+      <c r="L58" s="61"/>
+      <c r="M58" s="61"/>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="9">

</xml_diff>

<commit_message>
ok it does something just not much
</commit_message>
<xml_diff>
--- a/tests/testpwid.xlsx
+++ b/tests/testpwid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1712,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+    <sheetView topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2256,9 +2256,7 @@
       <c r="X19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y19" s="9">
-        <v>0</v>
-      </c>
+      <c r="Y19" s="9"/>
     </row>
     <row r="20" spans="1:25">
       <c r="B20" s="3" t="str">
@@ -2512,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3327,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12576,7 +12574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y85"/>
   <sheetViews>
-    <sheetView topLeftCell="K67" workbookViewId="0">
+    <sheetView topLeftCell="J56" workbookViewId="0">
       <selection activeCell="X83" sqref="X83:Y83"/>
     </sheetView>
   </sheetViews>

</xml_diff>